<commit_message>
add column indication do_d1 diameter ratios needed for Yo corrections
</commit_message>
<xml_diff>
--- a/errorbar_calculations/experiment_data_key.xlsx
+++ b/errorbar_calculations/experiment_data_key.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/changlvang/mygitFiles/diffusivity_calculations/errorbar_calculations/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/changvang/mygitFiles/diffusivity_calculations/errorbar_calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="35260" yWindow="5340" windowWidth="24560" windowHeight="14940"/>
+    <workbookView xWindow="9040" yWindow="4760" windowWidth="24560" windowHeight="14940"/>
   </bookViews>
   <sheets>
     <sheet name="HepHexPropGlyCSV" sheetId="13" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HepHexPropGlyCSV!$A$1:$U$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HepHexPropGlyCSV!$A$1:$W$54</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="93">
   <si>
     <t>No</t>
   </si>
@@ -303,12 +303,18 @@
   </si>
   <si>
     <t>Prop95/Gly5</t>
+  </si>
+  <si>
+    <t>t_fc</t>
+  </si>
+  <si>
+    <t>dod1_ratio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -507,7 +513,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -544,6 +550,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="129">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -749,6 +761,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1076,10 +1091,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U54"/>
+  <dimension ref="A1:W54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1088,19 +1103,19 @@
     <col min="2" max="2" width="13.5" style="1" customWidth="1"/>
     <col min="3" max="7" width="10.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="12.5" style="1" customWidth="1"/>
-    <col min="9" max="10" width="10.83203125" style="1" customWidth="1"/>
-    <col min="11" max="12" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.33203125" style="1" customWidth="1"/>
-    <col min="14" max="15" width="10.83203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.33203125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="10.83203125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="28.1640625" style="1" customWidth="1"/>
-    <col min="20" max="21" width="14.1640625" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="10.83203125" style="1"/>
+    <col min="9" max="12" width="10.83203125" style="1" customWidth="1"/>
+    <col min="13" max="14" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.33203125" style="1" customWidth="1"/>
+    <col min="16" max="17" width="10.83203125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.33203125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="10.83203125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="28.1640625" style="1" customWidth="1"/>
+    <col min="22" max="23" width="14.1640625" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>61</v>
       </c>
@@ -1129,43 +1144,49 @@
         <v>64</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1193,44 +1214,50 @@
       <c r="I2" s="5">
         <v>11.416700000000001</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="2">
+        <v>16</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1.0029220000000001</v>
+      </c>
+      <c r="L2" s="1">
         <v>2.3352003429019019</v>
       </c>
-      <c r="K2" s="1">
+      <c r="M2" s="1">
         <v>0.86542574294104924</v>
       </c>
-      <c r="L2" s="1">
+      <c r="N2" s="1">
         <v>3.0550000000000002</v>
       </c>
-      <c r="M2" s="1">
+      <c r="O2" s="1">
         <v>1.5599007653609722E-2</v>
       </c>
-      <c r="N2" s="2">
-        <v>1</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P2" s="3">
+      <c r="P2" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" s="3">
         <v>0.25</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="S2" s="3">
         <v>0.75</v>
       </c>
-      <c r="R2" s="3">
-        <v>0</v>
-      </c>
-      <c r="S2" s="4" t="s">
+      <c r="T2" s="3">
+        <v>0</v>
+      </c>
+      <c r="U2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1258,44 +1285,50 @@
       <c r="I3" s="5">
         <v>1.4</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1</v>
+      </c>
+      <c r="L3" s="1">
         <v>3.1782491106747073</v>
       </c>
-      <c r="K3" s="1">
+      <c r="M3" s="1">
         <v>0.31147821928890457</v>
       </c>
-      <c r="L3" s="1">
+      <c r="N3" s="1">
         <v>3.2570000000000001</v>
       </c>
-      <c r="M3" s="1">
+      <c r="O3" s="1">
         <v>0.23710700000000001</v>
       </c>
-      <c r="N3" s="3">
-        <v>1</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>1</v>
-      </c>
       <c r="P3" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R3" s="3">
         <v>0.25</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="S3" s="3">
         <v>0.75</v>
       </c>
-      <c r="R3" s="3">
-        <v>0</v>
-      </c>
-      <c r="S3" s="4" t="s">
+      <c r="T3" s="3">
+        <v>0</v>
+      </c>
+      <c r="U3" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="V3" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1323,44 +1356,50 @@
       <c r="I4" s="6">
         <v>1.2333000000000001</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="3">
+        <v>6</v>
+      </c>
+      <c r="K4" s="3">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1">
         <v>1.7595268527064873</v>
       </c>
-      <c r="K4" s="1">
+      <c r="M4" s="1">
         <v>0.87856072468684909</v>
       </c>
-      <c r="L4" s="1">
+      <c r="N4" s="1">
         <v>2.6739999999999999</v>
       </c>
-      <c r="M4" s="1">
+      <c r="O4" s="1">
         <v>1.8538767904454526E-2</v>
       </c>
-      <c r="N4" s="3">
-        <v>1</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>1</v>
-      </c>
       <c r="P4" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R4" s="3">
         <v>0.25</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="S4" s="3">
         <v>0.75</v>
       </c>
-      <c r="R4" s="3">
-        <v>0</v>
-      </c>
-      <c r="S4" s="4" t="s">
+      <c r="T4" s="3">
+        <v>0</v>
+      </c>
+      <c r="U4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T4" s="3" t="s">
+      <c r="V4" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="U4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1388,44 +1427,50 @@
       <c r="I5" s="6">
         <v>1.2</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1</v>
+      </c>
+      <c r="L5" s="1">
         <v>1.6226601615865228</v>
       </c>
-      <c r="K5" s="1">
+      <c r="M5" s="1">
         <v>0.88962479999999999</v>
       </c>
-      <c r="L5" s="1">
+      <c r="N5" s="1">
         <v>1.956</v>
       </c>
-      <c r="M5" s="1">
+      <c r="O5" s="1">
         <v>0.11561829999999999</v>
       </c>
-      <c r="N5" s="3">
-        <v>1</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>1</v>
-      </c>
       <c r="P5" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R5" s="3">
         <v>0.25</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="S5" s="3">
         <v>0.75</v>
       </c>
-      <c r="R5" s="3">
-        <v>0</v>
-      </c>
-      <c r="S5" s="4" t="s">
+      <c r="T5" s="3">
+        <v>0</v>
+      </c>
+      <c r="U5" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T5" s="3" t="s">
+      <c r="V5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="U5" s="3" t="s">
+      <c r="W5" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1453,44 +1498,50 @@
       <c r="I6" s="6">
         <v>1.3332999999999999</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="K6" s="3">
+        <v>1</v>
+      </c>
+      <c r="L6" s="1">
         <v>3.3308103570405705</v>
       </c>
-      <c r="K6" s="1">
+      <c r="M6" s="1">
         <v>0.77816955381709207</v>
       </c>
-      <c r="L6" s="1">
+      <c r="N6" s="1">
         <v>3.7469999999999999</v>
       </c>
-      <c r="M6" s="1">
+      <c r="O6" s="1">
         <v>1.3175665711066884E-2</v>
       </c>
-      <c r="N6" s="3">
-        <v>1</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>1</v>
-      </c>
       <c r="P6" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R6" s="3">
         <v>0.25</v>
       </c>
-      <c r="Q6" s="3">
+      <c r="S6" s="3">
         <v>0.75</v>
       </c>
-      <c r="R6" s="3">
-        <v>0</v>
-      </c>
-      <c r="S6" s="4" t="s">
+      <c r="T6" s="3">
+        <v>0</v>
+      </c>
+      <c r="U6" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T6" s="3" t="s">
+      <c r="V6" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="U6" s="3" t="s">
+      <c r="W6" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1518,44 +1569,50 @@
       <c r="I7" s="6">
         <v>1.5667</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="K7" s="3">
+        <v>1</v>
+      </c>
+      <c r="L7" s="1">
         <v>4.5427525411443783</v>
       </c>
-      <c r="K7" s="1">
+      <c r="M7" s="1">
         <v>0.57256821198903618</v>
       </c>
-      <c r="L7" s="1">
+      <c r="N7" s="1">
         <v>4.7670000000000003</v>
       </c>
-      <c r="M7" s="1">
+      <c r="O7" s="1">
         <v>1.0189170981642985E-2</v>
       </c>
-      <c r="N7" s="3">
-        <v>1</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>1</v>
-      </c>
       <c r="P7" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R7" s="3">
         <v>0.25</v>
       </c>
-      <c r="Q7" s="3">
+      <c r="S7" s="3">
         <v>0.75</v>
       </c>
-      <c r="R7" s="3">
-        <v>0</v>
-      </c>
-      <c r="S7" s="4" t="s">
+      <c r="T7" s="3">
+        <v>0</v>
+      </c>
+      <c r="U7" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T7" s="3" t="s">
+      <c r="V7" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="U7" s="3" t="s">
+      <c r="W7" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
@@ -1583,44 +1640,50 @@
       <c r="I8" s="6">
         <v>4.1166999999999998</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="3">
+        <v>12.22</v>
+      </c>
+      <c r="K8" s="3">
+        <v>1.000224</v>
+      </c>
+      <c r="L8" s="1">
         <v>1.8895348592146692</v>
       </c>
-      <c r="K8" s="1">
+      <c r="M8" s="1">
         <v>0.99756129747618505</v>
       </c>
-      <c r="L8" s="1">
+      <c r="N8" s="1">
         <v>3.3410000000000002</v>
       </c>
-      <c r="M8" s="1">
+      <c r="O8" s="1">
         <v>3.7223011081678678E-2</v>
       </c>
-      <c r="N8" s="3">
-        <v>1</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>0</v>
-      </c>
       <c r="P8" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R8" s="3">
         <v>0.4</v>
       </c>
-      <c r="Q8" s="3">
+      <c r="S8" s="3">
         <v>0.6</v>
       </c>
-      <c r="R8" s="3">
-        <v>0</v>
-      </c>
-      <c r="S8" s="4" t="s">
+      <c r="T8" s="3">
+        <v>0</v>
+      </c>
+      <c r="U8" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T8" s="3" t="s">
+      <c r="V8" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="U8" s="3" t="s">
+      <c r="W8" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>32</v>
       </c>
@@ -1648,44 +1711,50 @@
       <c r="I9" s="6">
         <v>6.4166999999999996</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="3">
+        <v>15</v>
+      </c>
+      <c r="K9" s="3">
+        <v>1.000345</v>
+      </c>
+      <c r="L9" s="1">
         <v>1.8969479519148542</v>
       </c>
-      <c r="K9" s="1">
+      <c r="M9" s="1">
         <v>1.01357446734192</v>
       </c>
-      <c r="L9" s="1">
+      <c r="N9" s="1">
         <v>3.444</v>
       </c>
-      <c r="M9" s="1">
+      <c r="O9" s="1">
         <v>0.1058259</v>
       </c>
-      <c r="N9" s="3">
-        <v>1</v>
-      </c>
-      <c r="O9" s="4" t="s">
-        <v>0</v>
-      </c>
       <c r="P9" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R9" s="3">
         <v>0.4</v>
       </c>
-      <c r="Q9" s="3">
+      <c r="S9" s="3">
         <v>0.6</v>
       </c>
-      <c r="R9" s="3">
-        <v>0</v>
-      </c>
-      <c r="S9" s="4" t="s">
+      <c r="T9" s="3">
+        <v>0</v>
+      </c>
+      <c r="U9" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T9" s="3" t="s">
+      <c r="V9" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="U9" s="3" t="s">
+      <c r="W9" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>33</v>
       </c>
@@ -1713,44 +1782,50 @@
       <c r="I10" s="6">
         <v>6.65</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="3">
+        <v>23.4</v>
+      </c>
+      <c r="K10" s="3">
+        <v>1.0005230000000001</v>
+      </c>
+      <c r="L10" s="1">
         <v>2.3805172953507627</v>
       </c>
-      <c r="K10" s="1">
+      <c r="M10" s="1">
         <v>0.92819728428385595</v>
       </c>
-      <c r="L10" s="1">
+      <c r="N10" s="1">
         <v>4.577</v>
       </c>
-      <c r="M10" s="1">
+      <c r="O10" s="1">
         <v>1.7337524421788E-2</v>
       </c>
-      <c r="N10" s="3">
-        <v>1</v>
-      </c>
-      <c r="O10" s="4" t="s">
-        <v>0</v>
-      </c>
       <c r="P10" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R10" s="3">
         <v>0.4</v>
       </c>
-      <c r="Q10" s="3">
+      <c r="S10" s="3">
         <v>0.6</v>
       </c>
-      <c r="R10" s="3">
-        <v>0</v>
-      </c>
-      <c r="S10" s="4" t="s">
+      <c r="T10" s="3">
+        <v>0</v>
+      </c>
+      <c r="U10" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T10" s="3" t="s">
+      <c r="V10" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="U10" s="3" t="s">
+      <c r="W10" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>34</v>
       </c>
@@ -1778,44 +1853,50 @@
       <c r="I11" s="6">
         <v>5.9667000000000003</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="3">
+        <v>23.2</v>
+      </c>
+      <c r="K11" s="3">
+        <v>1.00054</v>
+      </c>
+      <c r="L11" s="1">
         <v>2.4465859985387741</v>
       </c>
-      <c r="K11" s="1">
+      <c r="M11" s="1">
         <v>0.93654537878516297</v>
       </c>
-      <c r="L11" s="1">
+      <c r="N11" s="1">
         <v>4.6109999999999998</v>
       </c>
-      <c r="M11" s="1">
+      <c r="O11" s="1">
         <v>1.416773E-2</v>
       </c>
-      <c r="N11" s="2">
-        <v>1</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="P11" s="3">
+      <c r="P11" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R11" s="3">
         <v>0.4</v>
       </c>
-      <c r="Q11" s="3">
+      <c r="S11" s="3">
         <v>0.6</v>
       </c>
-      <c r="R11" s="3">
-        <v>0</v>
-      </c>
-      <c r="S11" s="4" t="s">
+      <c r="T11" s="3">
+        <v>0</v>
+      </c>
+      <c r="U11" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T11" s="3" t="s">
+      <c r="V11" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="U11" s="3" t="s">
+      <c r="W11" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>35</v>
       </c>
@@ -1843,44 +1924,50 @@
       <c r="I12" s="6">
         <v>6.1166999999999998</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12" s="3">
+        <v>15</v>
+      </c>
+      <c r="K12" s="3">
+        <v>1.000732</v>
+      </c>
+      <c r="L12" s="1">
         <v>2.0050525896258056</v>
       </c>
-      <c r="K12" s="1">
+      <c r="M12" s="1">
         <v>0.98639234064819004</v>
       </c>
-      <c r="L12" s="1">
+      <c r="N12" s="1">
         <v>3.5259999999999998</v>
       </c>
-      <c r="M12" s="1">
+      <c r="O12" s="1">
         <v>1.0788930429595204E-2</v>
       </c>
-      <c r="N12" s="2">
-        <v>1</v>
-      </c>
-      <c r="O12" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="P12" s="3">
+      <c r="P12" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R12" s="3">
         <v>0.4</v>
       </c>
-      <c r="Q12" s="3">
+      <c r="S12" s="3">
         <v>0.6</v>
       </c>
-      <c r="R12" s="3">
-        <v>0</v>
-      </c>
-      <c r="S12" s="4" t="s">
+      <c r="T12" s="3">
+        <v>0</v>
+      </c>
+      <c r="U12" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T12" s="3" t="s">
+      <c r="V12" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="U12" s="3" t="s">
+      <c r="W12" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -1908,44 +1995,50 @@
       <c r="I13" s="6">
         <v>6.9667000000000003</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13" s="3">
+        <v>16</v>
+      </c>
+      <c r="K13" s="3">
+        <v>1</v>
+      </c>
+      <c r="L13" s="1">
         <v>1.7207300834238937</v>
       </c>
-      <c r="K13" s="1">
+      <c r="M13" s="1">
         <v>1.111385021547</v>
       </c>
-      <c r="L13" s="1">
+      <c r="N13" s="1">
         <v>3.4</v>
       </c>
-      <c r="M13" s="1">
+      <c r="O13" s="1">
         <v>6.5035720000000005E-2</v>
       </c>
-      <c r="N13" s="2">
+      <c r="P13" s="2">
         <v>3</v>
       </c>
-      <c r="O13" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="P13" s="3">
+      <c r="Q13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R13" s="3">
         <v>0.4</v>
       </c>
-      <c r="Q13" s="3">
+      <c r="S13" s="3">
         <v>0.6</v>
       </c>
-      <c r="R13" s="3">
-        <v>0</v>
-      </c>
-      <c r="S13" s="4" t="s">
+      <c r="T13" s="3">
+        <v>0</v>
+      </c>
+      <c r="U13" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T13" s="3" t="s">
+      <c r="V13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="U13" s="3" t="s">
+      <c r="W13" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -1973,44 +2066,50 @@
       <c r="I14" s="5">
         <v>1.9333</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J14" s="2">
+        <v>5.9</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1</v>
+      </c>
+      <c r="L14" s="1">
         <v>0.90029601864157494</v>
       </c>
-      <c r="K14" s="1">
+      <c r="M14" s="1">
         <v>1.2827282942197</v>
       </c>
-      <c r="L14" s="1">
+      <c r="N14" s="1">
         <v>2.2709999999999999</v>
       </c>
-      <c r="M14" s="1">
+      <c r="O14" s="1">
         <v>0.14155158246268626</v>
       </c>
-      <c r="N14" s="2">
+      <c r="P14" s="2">
         <v>3</v>
       </c>
-      <c r="O14" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="P14" s="3">
+      <c r="Q14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R14" s="3">
         <v>0.4</v>
       </c>
-      <c r="Q14" s="3">
+      <c r="S14" s="3">
         <v>0.6</v>
       </c>
-      <c r="R14" s="3">
-        <v>0</v>
-      </c>
-      <c r="S14" s="4" t="s">
+      <c r="T14" s="3">
+        <v>0</v>
+      </c>
+      <c r="U14" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T14" s="3" t="s">
+      <c r="V14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="U14" s="3" t="s">
+      <c r="W14" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -2038,44 +2137,50 @@
       <c r="I15" s="5">
         <v>1.4</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J15" s="2">
+        <v>4.234</v>
+      </c>
+      <c r="K15" s="2">
+        <v>1</v>
+      </c>
+      <c r="L15" s="1">
         <v>0.74911973028330658</v>
       </c>
-      <c r="K15" s="1">
+      <c r="M15" s="1">
         <v>1.1181504896838499</v>
       </c>
-      <c r="L15" s="1">
+      <c r="N15" s="1">
         <v>1.8520000000000001</v>
       </c>
-      <c r="M15" s="1">
+      <c r="O15" s="1">
         <v>0.11419509999999999</v>
       </c>
-      <c r="N15" s="2">
+      <c r="P15" s="2">
         <v>3</v>
       </c>
-      <c r="O15" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P15" s="3">
+      <c r="Q15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R15" s="3">
         <v>0.4</v>
       </c>
-      <c r="Q15" s="3">
+      <c r="S15" s="3">
         <v>0.6</v>
       </c>
-      <c r="R15" s="3">
-        <v>0</v>
-      </c>
-      <c r="S15" s="4" t="s">
+      <c r="T15" s="3">
+        <v>0</v>
+      </c>
+      <c r="U15" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T15" s="3" t="s">
+      <c r="V15" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="U15" s="3" t="s">
+      <c r="W15" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -2103,44 +2208,50 @@
       <c r="I16" s="5">
         <v>11</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J16" s="2">
+        <v>27.2</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1.0003439999999999</v>
+      </c>
+      <c r="L16" s="1">
         <v>2.9690861903124959</v>
       </c>
-      <c r="K16" s="1">
+      <c r="M16" s="1">
         <v>1.0310635333812701</v>
       </c>
-      <c r="L16" s="1">
+      <c r="N16" s="1">
         <v>4.3259999999999996</v>
       </c>
-      <c r="M16" s="1">
+      <c r="O16" s="1">
         <v>2.1894589999999998E-2</v>
       </c>
-      <c r="N16" s="2">
+      <c r="P16" s="2">
         <v>3</v>
       </c>
-      <c r="O16" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P16" s="3">
+      <c r="Q16" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R16" s="3">
         <v>0.4</v>
       </c>
-      <c r="Q16" s="3">
+      <c r="S16" s="3">
         <v>0.6</v>
       </c>
-      <c r="R16" s="3">
-        <v>0</v>
-      </c>
-      <c r="S16" s="4" t="s">
+      <c r="T16" s="3">
+        <v>0</v>
+      </c>
+      <c r="U16" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T16" s="3" t="s">
+      <c r="V16" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="U16" s="3" t="s">
+      <c r="W16" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
@@ -2168,44 +2279,50 @@
       <c r="I17" s="5">
         <v>1.4</v>
       </c>
-      <c r="J17" s="1">
+      <c r="J17" s="2">
+        <v>5</v>
+      </c>
+      <c r="K17" s="2">
+        <v>1</v>
+      </c>
+      <c r="L17" s="1">
         <v>1.3013672282689579</v>
       </c>
-      <c r="K17" s="1">
+      <c r="M17" s="1">
         <v>0.87239454488214396</v>
       </c>
-      <c r="L17" s="1">
+      <c r="N17" s="1">
         <v>2.1800000000000002</v>
       </c>
-      <c r="M17" s="1">
+      <c r="O17" s="1">
         <v>3.3356180411974801E-2</v>
       </c>
-      <c r="N17" s="2">
+      <c r="P17" s="2">
         <v>3</v>
       </c>
-      <c r="O17" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="P17" s="3">
+      <c r="Q17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R17" s="3">
         <v>0.25</v>
       </c>
-      <c r="Q17" s="3">
+      <c r="S17" s="3">
         <v>0.75</v>
       </c>
-      <c r="R17" s="3">
-        <v>0</v>
-      </c>
-      <c r="S17" s="4" t="s">
+      <c r="T17" s="3">
+        <v>0</v>
+      </c>
+      <c r="U17" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T17" s="3" t="s">
+      <c r="V17" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="U17" s="3" t="s">
+      <c r="W17" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -2233,44 +2350,50 @@
       <c r="I18" s="5">
         <v>6.6</v>
       </c>
-      <c r="J18" s="1">
+      <c r="J18" s="2">
+        <v>9.5</v>
+      </c>
+      <c r="K18" s="2">
+        <v>1.0010840000000001</v>
+      </c>
+      <c r="L18" s="1">
         <v>1.3432809715324714</v>
       </c>
-      <c r="K18" s="1">
+      <c r="M18" s="1">
         <v>1.0251664401121099</v>
       </c>
-      <c r="L18" s="1">
+      <c r="N18" s="1">
         <v>2.14</v>
       </c>
-      <c r="M18" s="1">
+      <c r="O18" s="1">
         <v>0.11140410000000001</v>
       </c>
-      <c r="N18" s="2">
+      <c r="P18" s="2">
         <v>3</v>
       </c>
-      <c r="O18" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P18" s="3">
+      <c r="Q18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R18" s="3">
         <v>0.25</v>
       </c>
-      <c r="Q18" s="3">
+      <c r="S18" s="3">
         <v>0.75</v>
       </c>
-      <c r="R18" s="3">
-        <v>0</v>
-      </c>
-      <c r="S18" s="4" t="s">
+      <c r="T18" s="3">
+        <v>0</v>
+      </c>
+      <c r="U18" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T18" s="3" t="s">
+      <c r="V18" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="U18" s="3" t="s">
+      <c r="W18" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -2298,44 +2421,50 @@
       <c r="I19" s="5">
         <v>10.683299999999999</v>
       </c>
-      <c r="J19" s="1">
+      <c r="J19" s="2">
+        <v>15</v>
+      </c>
+      <c r="K19" s="2">
+        <v>1.001134</v>
+      </c>
+      <c r="L19" s="1">
         <v>3.2957485024392108</v>
       </c>
-      <c r="K19" s="1">
+      <c r="M19" s="1">
         <v>0.94391427224330404</v>
       </c>
-      <c r="L19" s="1">
+      <c r="N19" s="1">
         <v>3.7010000000000001</v>
       </c>
-      <c r="M19" s="1">
+      <c r="O19" s="1">
         <v>3.3196065079721428E-2</v>
       </c>
-      <c r="N19" s="2">
+      <c r="P19" s="2">
         <v>3</v>
       </c>
-      <c r="O19" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P19" s="3">
+      <c r="Q19" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R19" s="3">
         <v>0.25</v>
       </c>
-      <c r="Q19" s="3">
+      <c r="S19" s="3">
         <v>0.75</v>
       </c>
-      <c r="R19" s="3">
-        <v>0</v>
-      </c>
-      <c r="S19" s="4" t="s">
+      <c r="T19" s="3">
+        <v>0</v>
+      </c>
+      <c r="U19" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T19" s="3" t="s">
+      <c r="V19" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="U19" s="3" t="s">
+      <c r="W19" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -2363,44 +2492,50 @@
       <c r="I20" s="5">
         <v>4.1333000000000002</v>
       </c>
-      <c r="J20" s="1">
+      <c r="J20" s="2">
+        <v>12</v>
+      </c>
+      <c r="K20" s="2">
+        <v>1.0004409999999999</v>
+      </c>
+      <c r="L20" s="1">
         <v>2.5995343112307423</v>
       </c>
-      <c r="K20" s="1">
+      <c r="M20" s="1">
         <v>0.83882830336431902</v>
       </c>
-      <c r="L20" s="1">
+      <c r="N20" s="1">
         <v>3.61</v>
       </c>
-      <c r="M20" s="1">
+      <c r="O20" s="1">
         <v>1.2178062442019449E-2</v>
       </c>
-      <c r="N20" s="2">
-        <v>1</v>
-      </c>
-      <c r="O20" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="P20" s="3">
+      <c r="P20" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R20" s="3">
         <v>0.25</v>
       </c>
-      <c r="Q20" s="3">
+      <c r="S20" s="3">
         <v>0.75</v>
       </c>
-      <c r="R20" s="3">
-        <v>0</v>
-      </c>
-      <c r="S20" s="4" t="s">
+      <c r="T20" s="3">
+        <v>0</v>
+      </c>
+      <c r="U20" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T20" s="3" t="s">
+      <c r="V20" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="U20" s="3" t="s">
+      <c r="W20" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
@@ -2428,44 +2563,50 @@
       <c r="I21" s="5">
         <v>4.1833</v>
       </c>
-      <c r="J21" s="1">
+      <c r="J21" s="2">
+        <v>9.5</v>
+      </c>
+      <c r="K21" s="2">
+        <v>1.0008429999999999</v>
+      </c>
+      <c r="L21" s="1">
         <v>1.5609005233551816</v>
       </c>
-      <c r="K21" s="1">
+      <c r="M21" s="1">
         <v>0.83306795860358696</v>
       </c>
-      <c r="L21" s="1">
+      <c r="N21" s="1">
         <v>2.6459999999999999</v>
       </c>
-      <c r="M21" s="1">
+      <c r="O21" s="1">
         <v>1.7502309794915318E-2</v>
       </c>
-      <c r="N21" s="2">
-        <v>1</v>
-      </c>
-      <c r="O21" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="P21" s="3">
+      <c r="P21" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R21" s="3">
         <v>0.25</v>
       </c>
-      <c r="Q21" s="3">
+      <c r="S21" s="3">
         <v>0.75</v>
       </c>
-      <c r="R21" s="3">
-        <v>0</v>
-      </c>
-      <c r="S21" s="4" t="s">
+      <c r="T21" s="3">
+        <v>0</v>
+      </c>
+      <c r="U21" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T21" s="3" t="s">
+      <c r="V21" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="U21" s="3" t="s">
+      <c r="W21" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -2493,44 +2634,50 @@
       <c r="I22" s="5">
         <v>4.6333000000000002</v>
       </c>
-      <c r="J22" s="1">
+      <c r="J22" s="2">
+        <v>11.5</v>
+      </c>
+      <c r="K22" s="2">
+        <v>1.0000640000000001</v>
+      </c>
+      <c r="L22" s="1">
         <v>2.7212923982490453</v>
       </c>
-      <c r="K22" s="1">
+      <c r="M22" s="1">
         <v>0.70058610803839805</v>
       </c>
-      <c r="L22" s="1">
+      <c r="N22" s="1">
         <v>3.9079999999999999</v>
       </c>
-      <c r="M22" s="1">
+      <c r="O22" s="1">
         <v>5.1131999999999997E-2</v>
       </c>
-      <c r="N22" s="2">
-        <v>1</v>
-      </c>
-      <c r="O22" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="P22" s="3">
+      <c r="P22" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R22" s="3">
         <v>0.25</v>
       </c>
-      <c r="Q22" s="3">
+      <c r="S22" s="3">
         <v>0.75</v>
       </c>
-      <c r="R22" s="3">
-        <v>0</v>
-      </c>
-      <c r="S22" s="4" t="s">
+      <c r="T22" s="3">
+        <v>0</v>
+      </c>
+      <c r="U22" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T22" s="3" t="s">
+      <c r="V22" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="U22" s="3" t="s">
+      <c r="W22" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -2558,44 +2705,50 @@
       <c r="I23" s="5">
         <v>6.3833000000000002</v>
       </c>
-      <c r="J23" s="1">
+      <c r="J23" s="2">
+        <v>14.8</v>
+      </c>
+      <c r="K23" s="2">
+        <v>1.0021519999999999</v>
+      </c>
+      <c r="L23" s="1">
         <v>1.9494412846554856</v>
       </c>
-      <c r="K23" s="1">
+      <c r="M23" s="1">
         <v>0.19549291788415901</v>
       </c>
-      <c r="L23" s="1">
+      <c r="N23" s="1">
         <v>2.5550000000000002</v>
       </c>
-      <c r="M23" s="1">
+      <c r="O23" s="1">
         <v>6.7645120000000003E-2</v>
       </c>
-      <c r="N23" s="2">
-        <v>1</v>
-      </c>
-      <c r="O23" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P23" s="3">
+      <c r="P23" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R23" s="3">
         <v>0.2</v>
       </c>
-      <c r="Q23" s="3">
-        <v>0</v>
-      </c>
-      <c r="R23" s="3">
+      <c r="S23" s="3">
+        <v>0</v>
+      </c>
+      <c r="T23" s="3">
         <v>0.8</v>
       </c>
-      <c r="S23" s="4" t="s">
+      <c r="U23" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="T23" s="3" t="s">
+      <c r="V23" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="U23" s="3" t="s">
+      <c r="W23" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
@@ -2623,44 +2776,50 @@
       <c r="I24" s="5">
         <v>1.3332999999999999</v>
       </c>
-      <c r="J24" s="1">
+      <c r="J24" s="2">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="K24" s="2">
+        <v>1</v>
+      </c>
+      <c r="L24" s="1">
         <v>1.3493456211811117</v>
       </c>
-      <c r="K24" s="1">
+      <c r="M24" s="1">
         <v>0.48513270192097302</v>
       </c>
-      <c r="L24" s="1">
+      <c r="N24" s="1">
         <v>2.4489999999999998</v>
       </c>
-      <c r="M24" s="1">
+      <c r="O24" s="1">
         <v>2.4227052027731628E-2</v>
       </c>
-      <c r="N24" s="2">
-        <v>1</v>
-      </c>
-      <c r="O24" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P24" s="3">
+      <c r="P24" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R24" s="3">
         <v>0.2</v>
       </c>
-      <c r="Q24" s="3">
-        <v>0</v>
-      </c>
-      <c r="R24" s="3">
+      <c r="S24" s="3">
+        <v>0</v>
+      </c>
+      <c r="T24" s="3">
         <v>0.8</v>
       </c>
-      <c r="S24" s="4" t="s">
+      <c r="U24" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="T24" s="3" t="s">
+      <c r="V24" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="U24" s="3" t="s">
+      <c r="W24" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
@@ -2688,44 +2847,50 @@
       <c r="I25" s="5">
         <v>1.1333</v>
       </c>
-      <c r="J25" s="1">
+      <c r="J25" s="2">
+        <v>9.7669999999999995</v>
+      </c>
+      <c r="K25" s="2">
+        <v>1</v>
+      </c>
+      <c r="L25" s="1">
         <v>1.2635864382779676</v>
       </c>
-      <c r="K25" s="1">
+      <c r="M25" s="1">
         <v>0.46613965099999999</v>
       </c>
-      <c r="L25" s="1">
+      <c r="N25" s="1">
         <v>2.302</v>
       </c>
-      <c r="M25" s="1">
+      <c r="O25" s="1">
         <v>4.3412705839991267E-2</v>
       </c>
-      <c r="N25" s="2">
-        <v>1</v>
-      </c>
-      <c r="O25" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="P25" s="3">
+      <c r="P25" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R25" s="3">
         <v>0.2</v>
       </c>
-      <c r="Q25" s="3">
-        <v>0</v>
-      </c>
-      <c r="R25" s="3">
+      <c r="S25" s="3">
+        <v>0</v>
+      </c>
+      <c r="T25" s="3">
         <v>0.8</v>
       </c>
-      <c r="S25" s="4" t="s">
+      <c r="U25" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="T25" s="3" t="s">
+      <c r="V25" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="U25" s="3" t="s">
+      <c r="W25" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
@@ -2753,44 +2918,50 @@
       <c r="I26" s="5">
         <v>1</v>
       </c>
-      <c r="J26" s="1">
+      <c r="J26" s="2">
+        <v>11.5</v>
+      </c>
+      <c r="K26" s="2">
+        <v>1</v>
+      </c>
+      <c r="L26" s="1">
         <v>3.3192755723100786</v>
       </c>
-      <c r="K26" s="1">
+      <c r="M26" s="1">
         <v>0.40431680917130303</v>
       </c>
-      <c r="L26" s="1">
+      <c r="N26" s="1">
         <v>3.8029999999999999</v>
       </c>
-      <c r="M26" s="1">
+      <c r="O26" s="1">
         <v>4.3512275306778958E-3</v>
       </c>
-      <c r="N26" s="2">
-        <v>1</v>
-      </c>
-      <c r="O26" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="P26" s="3">
+      <c r="P26" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R26" s="3">
         <v>0.2</v>
       </c>
-      <c r="Q26" s="3">
-        <v>0</v>
-      </c>
-      <c r="R26" s="3">
+      <c r="S26" s="3">
+        <v>0</v>
+      </c>
+      <c r="T26" s="3">
         <v>0.8</v>
       </c>
-      <c r="S26" s="4" t="s">
+      <c r="U26" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="T26" s="3" t="s">
+      <c r="V26" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="U26" s="3" t="s">
+      <c r="W26" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
@@ -2818,44 +2989,50 @@
       <c r="I27" s="5">
         <v>18.283300000000001</v>
       </c>
-      <c r="J27" s="1">
+      <c r="J27" s="2">
+        <v>28.5</v>
+      </c>
+      <c r="K27" s="2">
+        <v>1.0030049999999999</v>
+      </c>
+      <c r="L27" s="1">
         <v>3.2584591687434568</v>
       </c>
-      <c r="K27" s="1">
+      <c r="M27" s="1">
         <v>0.42619913669655801</v>
       </c>
-      <c r="L27" s="1">
+      <c r="N27" s="1">
         <v>3.786</v>
       </c>
-      <c r="M27" s="1">
+      <c r="O27" s="1">
         <v>1.3635522871068416E-2</v>
       </c>
-      <c r="N27" s="2">
-        <v>1</v>
-      </c>
-      <c r="O27" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P27" s="3">
+      <c r="P27" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R27" s="3">
         <v>0.2</v>
       </c>
-      <c r="Q27" s="3">
-        <v>0</v>
-      </c>
-      <c r="R27" s="3">
+      <c r="S27" s="3">
+        <v>0</v>
+      </c>
+      <c r="T27" s="3">
         <v>0.8</v>
       </c>
-      <c r="S27" s="4" t="s">
+      <c r="U27" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="T27" s="3" t="s">
+      <c r="V27" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="U27" s="3" t="s">
+      <c r="W27" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
@@ -2883,44 +3060,50 @@
       <c r="I28" s="5">
         <v>4.5332999999999997</v>
       </c>
-      <c r="J28" s="1">
+      <c r="J28" s="2">
+        <v>16</v>
+      </c>
+      <c r="K28" s="2">
+        <v>1</v>
+      </c>
+      <c r="L28" s="1">
         <v>1.4721342978356493</v>
       </c>
-      <c r="K28" s="1">
+      <c r="M28" s="1">
         <v>0.61127582914535905</v>
       </c>
-      <c r="L28" s="1">
+      <c r="N28" s="1">
         <v>2.9</v>
       </c>
-      <c r="M28" s="1">
+      <c r="O28" s="1">
         <v>8.6762317607479052E-3</v>
       </c>
-      <c r="N28" s="2">
-        <v>1</v>
-      </c>
-      <c r="O28" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="P28" s="3">
+      <c r="P28" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R28" s="3">
         <v>0.3</v>
       </c>
-      <c r="Q28" s="3">
-        <v>0</v>
-      </c>
-      <c r="R28" s="3">
+      <c r="S28" s="3">
+        <v>0</v>
+      </c>
+      <c r="T28" s="3">
         <v>0.7</v>
       </c>
-      <c r="S28" s="4" t="s">
+      <c r="U28" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="T28" s="3" t="s">
+      <c r="V28" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="U28" s="3" t="s">
+      <c r="W28" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
@@ -2948,44 +3131,50 @@
       <c r="I29" s="5">
         <v>4.1833</v>
       </c>
-      <c r="J29" s="1">
+      <c r="J29" s="2">
+        <v>21.9</v>
+      </c>
+      <c r="K29" s="2">
+        <v>1</v>
+      </c>
+      <c r="L29" s="1">
         <v>1.7783994540035148</v>
       </c>
-      <c r="K29" s="1">
+      <c r="M29" s="1">
         <v>0.55735224048967502</v>
       </c>
-      <c r="L29" s="1">
+      <c r="N29" s="1">
         <v>3.4740000000000002</v>
       </c>
-      <c r="M29" s="1">
+      <c r="O29" s="1">
         <v>6.2538634629654248E-3</v>
       </c>
-      <c r="N29" s="2">
-        <v>1</v>
-      </c>
-      <c r="O29" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="P29" s="3">
+      <c r="P29" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R29" s="3">
         <v>0.3</v>
       </c>
-      <c r="Q29" s="3">
-        <v>0</v>
-      </c>
-      <c r="R29" s="3">
+      <c r="S29" s="3">
+        <v>0</v>
+      </c>
+      <c r="T29" s="3">
         <v>0.7</v>
       </c>
-      <c r="S29" s="4" t="s">
+      <c r="U29" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="T29" s="3" t="s">
+      <c r="V29" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="U29" s="3" t="s">
+      <c r="W29" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
@@ -3013,44 +3202,50 @@
       <c r="I30" s="5">
         <v>4.2</v>
       </c>
-      <c r="J30" s="1">
+      <c r="J30" s="2">
+        <v>15</v>
+      </c>
+      <c r="K30" s="2">
+        <v>1.0002800000000001</v>
+      </c>
+      <c r="L30" s="1">
         <v>1.5742704754901555</v>
       </c>
-      <c r="K30" s="1">
+      <c r="M30" s="1">
         <v>0.53949983000000001</v>
       </c>
-      <c r="L30" s="1">
+      <c r="N30" s="1">
         <v>2.855</v>
       </c>
-      <c r="M30" s="1">
+      <c r="O30" s="1">
         <v>9.7243943109169163E-3</v>
       </c>
-      <c r="N30" s="2">
-        <v>1</v>
-      </c>
-      <c r="O30" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="P30" s="3">
+      <c r="P30" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R30" s="3">
         <v>0.3</v>
       </c>
-      <c r="Q30" s="3">
-        <v>0</v>
-      </c>
-      <c r="R30" s="3">
+      <c r="S30" s="3">
+        <v>0</v>
+      </c>
+      <c r="T30" s="3">
         <v>0.7</v>
       </c>
-      <c r="S30" s="4" t="s">
+      <c r="U30" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="T30" s="3" t="s">
+      <c r="V30" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="U30" s="3" t="s">
+      <c r="W30" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
@@ -3078,44 +3273,50 @@
       <c r="I31" s="5">
         <v>4.1333000000000002</v>
       </c>
-      <c r="J31" s="1">
+      <c r="J31" s="2">
+        <v>16</v>
+      </c>
+      <c r="K31" s="2">
+        <v>1.000302</v>
+      </c>
+      <c r="L31" s="1">
         <v>1.7679228942462395</v>
       </c>
-      <c r="K31" s="1">
+      <c r="M31" s="1">
         <v>0.55187003199999995</v>
       </c>
-      <c r="L31" s="1">
+      <c r="N31" s="1">
         <v>3.0550000000000002</v>
       </c>
-      <c r="M31" s="1">
+      <c r="O31" s="1">
         <v>2.1945632660041521E-2</v>
       </c>
-      <c r="N31" s="2">
-        <v>1</v>
-      </c>
-      <c r="O31" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="P31" s="3">
+      <c r="P31" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R31" s="3">
         <v>0.3</v>
       </c>
-      <c r="Q31" s="3">
-        <v>0</v>
-      </c>
-      <c r="R31" s="3">
+      <c r="S31" s="3">
+        <v>0</v>
+      </c>
+      <c r="T31" s="3">
         <v>0.7</v>
       </c>
-      <c r="S31" s="4" t="s">
+      <c r="U31" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="T31" s="3" t="s">
+      <c r="V31" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="U31" s="3" t="s">
+      <c r="W31" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>37</v>
       </c>
@@ -3143,44 +3344,50 @@
       <c r="I32" s="5">
         <v>2.6833</v>
       </c>
-      <c r="J32" s="1">
+      <c r="J32" s="2">
+        <v>3.9</v>
+      </c>
+      <c r="K32" s="2">
+        <v>1.006756</v>
+      </c>
+      <c r="L32" s="1">
         <v>1.6968445001360319</v>
       </c>
-      <c r="K32" s="1">
+      <c r="M32" s="1">
         <v>0.85790774464492903</v>
       </c>
-      <c r="L32" s="1">
+      <c r="N32" s="1">
         <v>2.2149999999999999</v>
       </c>
-      <c r="M32" s="1">
+      <c r="O32" s="1">
         <v>5.7099184371145022E-2</v>
       </c>
-      <c r="N32" s="2">
-        <v>1</v>
-      </c>
-      <c r="O32" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P32" s="3">
+      <c r="P32" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R32" s="3">
         <v>0.3</v>
       </c>
-      <c r="Q32" s="3">
+      <c r="S32" s="3">
         <v>0.7</v>
       </c>
-      <c r="R32" s="3">
-        <v>0</v>
-      </c>
-      <c r="S32" s="4" t="s">
+      <c r="T32" s="3">
+        <v>0</v>
+      </c>
+      <c r="U32" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T32" s="3" t="s">
+      <c r="V32" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="U32" s="3" t="s">
+      <c r="W32" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>38</v>
       </c>
@@ -3208,44 +3415,50 @@
       <c r="I33" s="5">
         <v>4.0332999999999997</v>
       </c>
-      <c r="J33" s="1">
+      <c r="J33" s="2">
+        <v>5.59</v>
+      </c>
+      <c r="K33" s="2">
+        <v>1.0059720000000001</v>
+      </c>
+      <c r="L33" s="1">
         <v>0.92960986440549342</v>
       </c>
-      <c r="K33" s="1">
+      <c r="M33" s="1">
         <v>1.103988</v>
       </c>
-      <c r="L33" s="12">
+      <c r="N33" s="12">
         <v>1.7517416194523387</v>
       </c>
-      <c r="M33" s="1">
+      <c r="O33" s="1">
         <v>0.18659770000000001</v>
       </c>
-      <c r="N33" s="7">
-        <v>1</v>
-      </c>
-      <c r="O33" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P33" s="3">
+      <c r="P33" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R33" s="3">
         <v>0.4</v>
       </c>
-      <c r="Q33" s="3">
+      <c r="S33" s="3">
         <v>0.6</v>
       </c>
-      <c r="R33" s="3">
-        <v>0</v>
-      </c>
-      <c r="S33" s="4" t="s">
+      <c r="T33" s="3">
+        <v>0</v>
+      </c>
+      <c r="U33" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T33" s="3" t="s">
+      <c r="V33" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="U33" s="3" t="s">
+      <c r="W33" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>39</v>
       </c>
@@ -3273,44 +3486,50 @@
       <c r="I34" s="5">
         <v>9.15</v>
       </c>
-      <c r="J34" s="1">
+      <c r="J34" s="2">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="K34" s="2">
+        <v>1.0695410000000001</v>
+      </c>
+      <c r="L34" s="1">
         <v>1.6638361321570523</v>
       </c>
-      <c r="K34" s="1">
+      <c r="M34" s="1">
         <v>0.66226581990580402</v>
       </c>
-      <c r="L34" s="1">
+      <c r="N34" s="1">
         <v>2.0960000000000001</v>
       </c>
-      <c r="M34" s="1">
+      <c r="O34" s="1">
         <v>5.6947310000000001E-2</v>
       </c>
-      <c r="N34" s="2">
-        <v>1</v>
-      </c>
-      <c r="O34" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P34" s="3">
+      <c r="P34" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R34" s="3">
         <v>0.4</v>
       </c>
-      <c r="Q34" s="3">
+      <c r="S34" s="3">
         <v>0.6</v>
       </c>
-      <c r="R34" s="3">
-        <v>0</v>
-      </c>
-      <c r="S34" s="4" t="s">
+      <c r="T34" s="3">
+        <v>0</v>
+      </c>
+      <c r="U34" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T34" s="3" t="s">
+      <c r="V34" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="U34" s="3" t="s">
+      <c r="W34" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>40</v>
       </c>
@@ -3338,44 +3557,50 @@
       <c r="I35" s="5">
         <v>1.7833000000000001</v>
       </c>
-      <c r="J35" s="1">
+      <c r="J35" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="K35" s="2">
+        <v>1</v>
+      </c>
+      <c r="L35" s="1">
         <v>2.1810785044681036</v>
       </c>
-      <c r="K35" s="1">
+      <c r="M35" s="1">
         <v>0.98463900354119804</v>
       </c>
-      <c r="L35" s="1">
+      <c r="N35" s="1">
         <v>3.0710000000000002</v>
       </c>
-      <c r="M35" s="1">
+      <c r="O35" s="1">
         <v>5.9439330126580391E-2</v>
       </c>
-      <c r="N35" s="2">
-        <v>1</v>
-      </c>
-      <c r="O35" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P35" s="3">
+      <c r="P35" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R35" s="3">
         <v>0.4</v>
       </c>
-      <c r="Q35" s="3">
+      <c r="S35" s="3">
         <v>0.6</v>
       </c>
-      <c r="R35" s="3">
-        <v>0</v>
-      </c>
-      <c r="S35" s="4" t="s">
+      <c r="T35" s="3">
+        <v>0</v>
+      </c>
+      <c r="U35" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T35" s="3" t="s">
+      <c r="V35" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="U35" s="3" t="s">
+      <c r="W35" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>41</v>
       </c>
@@ -3403,44 +3628,50 @@
       <c r="I36" s="5">
         <v>19.033300000000001</v>
       </c>
-      <c r="J36" s="1">
+      <c r="J36" s="2">
+        <v>22.2</v>
+      </c>
+      <c r="K36" s="2">
+        <v>1.041544</v>
+      </c>
+      <c r="L36" s="1">
         <v>1.8099091137402452</v>
       </c>
-      <c r="K36" s="1">
+      <c r="M36" s="1">
         <v>1.160312</v>
       </c>
-      <c r="L36" s="1">
+      <c r="N36" s="1">
         <v>3.181</v>
       </c>
-      <c r="M36" s="1">
+      <c r="O36" s="1">
         <v>6.7135323553240644E-2</v>
       </c>
-      <c r="N36" s="2">
-        <v>1</v>
-      </c>
-      <c r="O36" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P36" s="3">
+      <c r="P36" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R36" s="3">
         <v>0.4</v>
       </c>
-      <c r="Q36" s="3">
+      <c r="S36" s="3">
         <v>0.6</v>
       </c>
-      <c r="R36" s="3">
-        <v>0</v>
-      </c>
-      <c r="S36" s="4" t="s">
+      <c r="T36" s="3">
+        <v>0</v>
+      </c>
+      <c r="U36" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T36" s="3" t="s">
+      <c r="V36" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="U36" s="3" t="s">
+      <c r="W36" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>42</v>
       </c>
@@ -3468,44 +3699,50 @@
       <c r="I37" s="5">
         <v>19.05</v>
       </c>
-      <c r="J37" s="1">
+      <c r="J37" s="2">
+        <v>22.1</v>
+      </c>
+      <c r="K37" s="2">
+        <v>1.0189699999999999</v>
+      </c>
+      <c r="L37" s="1">
         <v>2.0418631198001496</v>
       </c>
-      <c r="K37" s="1">
+      <c r="M37" s="1">
         <v>1.0603039999999999</v>
       </c>
-      <c r="L37" s="1">
+      <c r="N37" s="1">
         <v>2.9689999999999999</v>
       </c>
-      <c r="M37" s="1">
+      <c r="O37" s="1">
         <v>8.0571039999778493E-2</v>
       </c>
-      <c r="N37" s="2">
-        <v>1</v>
-      </c>
-      <c r="O37" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P37" s="3">
+      <c r="P37" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q37" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R37" s="3">
         <v>0.4</v>
       </c>
-      <c r="Q37" s="3">
+      <c r="S37" s="3">
         <v>0.6</v>
       </c>
-      <c r="R37" s="3">
-        <v>0</v>
-      </c>
-      <c r="S37" s="4" t="s">
+      <c r="T37" s="3">
+        <v>0</v>
+      </c>
+      <c r="U37" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T37" s="3" t="s">
+      <c r="V37" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="U37" s="3" t="s">
+      <c r="W37" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
         <v>43</v>
       </c>
@@ -3533,44 +3770,50 @@
       <c r="I38" s="5">
         <v>1.2666999999999999</v>
       </c>
-      <c r="J38" s="1">
+      <c r="J38" s="2">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="K38" s="2">
+        <v>1</v>
+      </c>
+      <c r="L38" s="1">
         <v>1.7134045056553342</v>
       </c>
-      <c r="K38" s="1">
+      <c r="M38" s="1">
         <v>0.58004920000000004</v>
       </c>
-      <c r="L38" s="1">
+      <c r="N38" s="1">
         <v>2.762</v>
       </c>
-      <c r="M38" s="1">
+      <c r="O38" s="1">
         <v>1.4792319999999999E-2</v>
       </c>
-      <c r="N38" s="7">
-        <v>1</v>
-      </c>
-      <c r="O38" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P38" s="3">
+      <c r="P38" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q38" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R38" s="3">
         <v>0.2</v>
       </c>
-      <c r="Q38" s="3">
-        <v>0</v>
-      </c>
-      <c r="R38" s="3">
+      <c r="S38" s="3">
+        <v>0</v>
+      </c>
+      <c r="T38" s="3">
         <v>0.8</v>
       </c>
-      <c r="S38" s="4" t="s">
+      <c r="U38" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="T38" s="3" t="s">
+      <c r="V38" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="U38" s="3" t="s">
+      <c r="W38" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>44</v>
       </c>
@@ -3598,44 +3841,50 @@
       <c r="I39" s="5">
         <v>8.8000000000000007</v>
       </c>
-      <c r="J39" s="1">
+      <c r="J39" s="2">
+        <v>13</v>
+      </c>
+      <c r="K39" s="2">
+        <v>1.0069520000000001</v>
+      </c>
+      <c r="L39" s="1">
         <v>1.4079360780944568</v>
       </c>
-      <c r="K39" s="1">
+      <c r="M39" s="1">
         <v>0.61468959999999995</v>
       </c>
-      <c r="L39" s="1">
+      <c r="N39" s="1">
         <v>2.0910000000000002</v>
       </c>
-      <c r="M39" s="1">
+      <c r="O39" s="1">
         <v>2.7755863304399921E-2</v>
       </c>
-      <c r="N39" s="2">
-        <v>1</v>
-      </c>
-      <c r="O39" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P39" s="3">
+      <c r="P39" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R39" s="3">
         <v>0.2</v>
       </c>
-      <c r="Q39" s="3">
-        <v>0</v>
-      </c>
-      <c r="R39" s="3">
+      <c r="S39" s="3">
+        <v>0</v>
+      </c>
+      <c r="T39" s="3">
         <v>0.8</v>
       </c>
-      <c r="S39" s="4" t="s">
+      <c r="U39" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="T39" s="3" t="s">
+      <c r="V39" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="U39" s="3" t="s">
+      <c r="W39" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>45</v>
       </c>
@@ -3663,44 +3912,50 @@
       <c r="I40" s="5">
         <v>1.1333</v>
       </c>
-      <c r="J40" s="1">
+      <c r="J40" s="2">
+        <v>22</v>
+      </c>
+      <c r="K40" s="2">
+        <v>1</v>
+      </c>
+      <c r="L40" s="1">
         <v>2.0322396512222665</v>
       </c>
-      <c r="K40" s="1">
+      <c r="M40" s="1">
         <v>0.42108139999999999</v>
       </c>
-      <c r="L40" s="1">
+      <c r="N40" s="1">
         <v>3.5569999999999999</v>
       </c>
-      <c r="M40" s="1">
+      <c r="O40" s="1">
         <v>4.5094499999999999E-3</v>
       </c>
-      <c r="N40" s="2">
-        <v>1</v>
-      </c>
-      <c r="O40" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P40" s="3">
+      <c r="P40" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q40" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R40" s="3">
         <v>0.2</v>
       </c>
-      <c r="Q40" s="3">
-        <v>0</v>
-      </c>
-      <c r="R40" s="3">
+      <c r="S40" s="3">
+        <v>0</v>
+      </c>
+      <c r="T40" s="3">
         <v>0.8</v>
       </c>
-      <c r="S40" s="4" t="s">
+      <c r="U40" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="T40" s="3" t="s">
+      <c r="V40" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="U40" s="3" t="s">
+      <c r="W40" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>47</v>
       </c>
@@ -3728,44 +3983,50 @@
       <c r="I41" s="5">
         <v>3.6</v>
       </c>
-      <c r="J41" s="1">
+      <c r="J41" s="2">
+        <v>8</v>
+      </c>
+      <c r="K41" s="2">
+        <v>1.0001949999999999</v>
+      </c>
+      <c r="L41" s="1">
         <v>3.5368435994127871</v>
       </c>
-      <c r="K41" s="13">
+      <c r="M41" s="13">
         <v>0.94141366120616898</v>
       </c>
-      <c r="L41" s="1">
+      <c r="N41" s="1">
         <v>4.1360000000000001</v>
       </c>
-      <c r="M41" s="1">
+      <c r="O41" s="1">
         <v>5.0657664752307305E-2</v>
       </c>
-      <c r="N41" s="2">
-        <v>1</v>
-      </c>
-      <c r="O41" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P41" s="3">
+      <c r="P41" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q41" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R41" s="3">
         <v>0.3</v>
       </c>
-      <c r="Q41" s="3">
+      <c r="S41" s="3">
         <v>0.7</v>
       </c>
-      <c r="R41" s="3">
-        <v>0</v>
-      </c>
-      <c r="S41" s="4" t="s">
+      <c r="T41" s="3">
+        <v>0</v>
+      </c>
+      <c r="U41" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T41" s="3" t="s">
+      <c r="V41" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="U41" s="3" t="s">
+      <c r="W41" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>48</v>
       </c>
@@ -3793,44 +4054,50 @@
       <c r="I42" s="9">
         <v>33.866700000000002</v>
       </c>
-      <c r="J42" s="11">
+      <c r="J42" s="14">
+        <v>36</v>
+      </c>
+      <c r="K42" s="14">
+        <v>1.0192270000000001</v>
+      </c>
+      <c r="L42" s="11">
         <v>3.491728798174337</v>
       </c>
-      <c r="K42" s="11">
+      <c r="M42" s="11">
         <v>0.64923280000000005</v>
       </c>
-      <c r="L42" s="11">
+      <c r="N42" s="11">
         <v>3.8210000000000002</v>
       </c>
-      <c r="M42" s="11">
+      <c r="O42" s="11">
         <v>3.1651350000000002E-2</v>
       </c>
-      <c r="N42" s="2">
-        <v>1</v>
-      </c>
-      <c r="O42" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P42" s="3">
+      <c r="P42" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q42" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R42" s="3">
         <v>0.3</v>
       </c>
-      <c r="Q42" s="3">
+      <c r="S42" s="3">
         <v>0.7</v>
       </c>
-      <c r="R42" s="3">
-        <v>0</v>
-      </c>
-      <c r="S42" s="4" t="s">
+      <c r="T42" s="3">
+        <v>0</v>
+      </c>
+      <c r="U42" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T42" s="3" t="s">
+      <c r="V42" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="U42" s="3" t="s">
+      <c r="W42" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>51</v>
       </c>
@@ -3858,44 +4125,50 @@
       <c r="I43" s="5">
         <v>2.0667</v>
       </c>
-      <c r="J43" s="1">
+      <c r="J43" s="2">
+        <v>2.6</v>
+      </c>
+      <c r="K43" s="2">
+        <v>1</v>
+      </c>
+      <c r="L43" s="1">
         <v>2.0605152574534142</v>
       </c>
-      <c r="K43" s="1">
+      <c r="M43" s="1">
         <v>0.62216463938926203</v>
       </c>
-      <c r="L43" s="1">
+      <c r="N43" s="1">
         <v>2.2610000000000001</v>
       </c>
-      <c r="M43" s="1">
+      <c r="O43" s="1">
         <v>0.12398128541251682</v>
       </c>
-      <c r="N43" s="2">
-        <v>1</v>
-      </c>
-      <c r="O43" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P43" s="3">
+      <c r="P43" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q43" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R43" s="3">
         <v>0.4</v>
       </c>
-      <c r="Q43" s="3">
+      <c r="S43" s="3">
         <v>0.6</v>
       </c>
-      <c r="R43" s="3">
-        <v>0</v>
-      </c>
-      <c r="S43" s="4" t="s">
+      <c r="T43" s="3">
+        <v>0</v>
+      </c>
+      <c r="U43" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T43" s="3" t="s">
+      <c r="V43" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="U43" s="3" t="s">
+      <c r="W43" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>50</v>
       </c>
@@ -3923,44 +4196,50 @@
       <c r="I44" s="5">
         <v>2.0333000000000001</v>
       </c>
-      <c r="J44" s="1">
+      <c r="J44" s="2">
+        <v>2.9</v>
+      </c>
+      <c r="K44" s="2">
+        <v>1</v>
+      </c>
+      <c r="L44" s="1">
         <v>2.13250457296486</v>
       </c>
-      <c r="K44" s="1">
+      <c r="M44" s="1">
         <v>0.81521320095990202</v>
       </c>
-      <c r="L44" s="1">
+      <c r="N44" s="1">
         <v>2.411</v>
       </c>
-      <c r="M44" s="1">
+      <c r="O44" s="1">
         <v>5.3186664357433709E-2</v>
       </c>
-      <c r="N44" s="2">
-        <v>1</v>
-      </c>
-      <c r="O44" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P44" s="3">
+      <c r="P44" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q44" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R44" s="3">
         <v>0.4</v>
       </c>
-      <c r="Q44" s="3">
+      <c r="S44" s="3">
         <v>0.6</v>
       </c>
-      <c r="R44" s="3">
-        <v>0</v>
-      </c>
-      <c r="S44" s="4" t="s">
+      <c r="T44" s="3">
+        <v>0</v>
+      </c>
+      <c r="U44" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T44" s="3" t="s">
+      <c r="V44" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="U44" s="3" t="s">
+      <c r="W44" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>49</v>
       </c>
@@ -3988,44 +4267,50 @@
       <c r="I45" s="10">
         <v>2.4666999999999999</v>
       </c>
-      <c r="J45" s="1">
+      <c r="J45" s="15">
+        <v>8.6</v>
+      </c>
+      <c r="K45" s="15">
+        <v>1</v>
+      </c>
+      <c r="L45" s="1">
         <v>3.2730050981108629</v>
       </c>
-      <c r="K45" s="11">
+      <c r="M45" s="11">
         <v>1.0649931910443</v>
       </c>
-      <c r="L45" s="11">
+      <c r="N45" s="11">
         <v>4.1790000000000003</v>
       </c>
-      <c r="M45" s="11">
+      <c r="O45" s="11">
         <v>0.1247629704105207</v>
       </c>
-      <c r="N45" s="2">
-        <v>1</v>
-      </c>
-      <c r="O45" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P45" s="3">
+      <c r="P45" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q45" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R45" s="3">
         <v>0.4</v>
       </c>
-      <c r="Q45" s="3">
+      <c r="S45" s="3">
         <v>0.6</v>
       </c>
-      <c r="R45" s="3">
-        <v>0</v>
-      </c>
-      <c r="S45" s="4" t="s">
+      <c r="T45" s="3">
+        <v>0</v>
+      </c>
+      <c r="U45" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T45" s="3" t="s">
+      <c r="V45" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="U45" s="3" t="s">
+      <c r="W45" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>52</v>
       </c>
@@ -4053,44 +4338,50 @@
       <c r="I46" s="9">
         <v>33.183300000000003</v>
       </c>
-      <c r="J46" s="1">
+      <c r="J46" s="14">
+        <v>39.5</v>
+      </c>
+      <c r="K46" s="14">
+        <v>1.018413</v>
+      </c>
+      <c r="L46" s="1">
         <v>3.356677737630632</v>
       </c>
-      <c r="K46" s="11">
+      <c r="M46" s="11">
         <v>0.99527808819216801</v>
       </c>
-      <c r="L46" s="11">
+      <c r="N46" s="11">
         <v>4.2949999999999999</v>
       </c>
-      <c r="M46" s="11">
+      <c r="O46" s="11">
         <v>3.7908100504388711E-2</v>
       </c>
-      <c r="N46" s="2">
-        <v>1</v>
-      </c>
-      <c r="O46" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P46" s="3">
+      <c r="P46" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q46" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R46" s="3">
         <v>0.4</v>
       </c>
-      <c r="Q46" s="3">
+      <c r="S46" s="3">
         <v>0.6</v>
       </c>
-      <c r="R46" s="3">
-        <v>0</v>
-      </c>
-      <c r="S46" s="4" t="s">
+      <c r="T46" s="3">
+        <v>0</v>
+      </c>
+      <c r="U46" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="T46" s="3" t="s">
+      <c r="V46" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="U46" s="3" t="s">
+      <c r="W46" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>53</v>
       </c>
@@ -4118,44 +4409,50 @@
       <c r="I47" s="5">
         <v>1.6</v>
       </c>
-      <c r="J47" s="1">
+      <c r="J47" s="2">
+        <v>2.9</v>
+      </c>
+      <c r="K47" s="2">
+        <v>1</v>
+      </c>
+      <c r="L47" s="1">
         <v>1.7594625712418352</v>
       </c>
-      <c r="K47" s="1">
+      <c r="M47" s="1">
         <v>0.33505653480486902</v>
       </c>
-      <c r="L47" s="1">
+      <c r="N47" s="1">
         <v>1.9079999999999999</v>
       </c>
-      <c r="M47" s="1">
+      <c r="O47" s="1">
         <v>6.5637906962917117E-2</v>
       </c>
-      <c r="N47" s="2">
-        <v>1</v>
-      </c>
-      <c r="O47" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P47" s="3">
+      <c r="P47" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q47" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R47" s="3">
         <v>0.2</v>
       </c>
-      <c r="Q47" s="3">
-        <v>0</v>
-      </c>
-      <c r="R47" s="3">
+      <c r="S47" s="3">
+        <v>0</v>
+      </c>
+      <c r="T47" s="3">
         <v>0.8</v>
       </c>
-      <c r="S47" s="4" t="s">
+      <c r="U47" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="T47" s="3" t="s">
+      <c r="V47" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="U47" s="3" t="s">
+      <c r="W47" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>54</v>
       </c>
@@ -4183,44 +4480,50 @@
       <c r="I48" s="5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J48" s="1">
+      <c r="J48" s="2">
+        <v>22</v>
+      </c>
+      <c r="K48" s="2">
+        <v>1</v>
+      </c>
+      <c r="L48" s="1">
         <v>2.8933112518358617</v>
       </c>
-      <c r="K48" s="1">
+      <c r="M48" s="1">
         <v>0.39015070000000002</v>
       </c>
-      <c r="L48" s="1">
+      <c r="N48" s="1">
         <v>3.9769999999999999</v>
       </c>
-      <c r="M48" s="1">
+      <c r="O48" s="1">
         <v>9.0218290000000003E-3</v>
       </c>
-      <c r="N48" s="2">
-        <v>1</v>
-      </c>
-      <c r="O48" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P48" s="3">
+      <c r="P48" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q48" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R48" s="3">
         <v>0.2</v>
       </c>
-      <c r="Q48" s="3">
-        <v>0</v>
-      </c>
-      <c r="R48" s="3">
+      <c r="S48" s="3">
+        <v>0</v>
+      </c>
+      <c r="T48" s="3">
         <v>0.8</v>
       </c>
-      <c r="S48" s="4" t="s">
+      <c r="U48" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="T48" s="3" t="s">
+      <c r="V48" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="U48" s="3" t="s">
+      <c r="W48" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>55</v>
       </c>
@@ -4248,44 +4551,50 @@
       <c r="I49" s="5">
         <v>8.8666999999999998</v>
       </c>
-      <c r="J49" s="1">
+      <c r="J49" s="2">
+        <v>11.2</v>
+      </c>
+      <c r="K49" s="2">
+        <v>1.0070410000000001</v>
+      </c>
+      <c r="L49" s="1">
         <v>1.8843110905231282</v>
       </c>
-      <c r="K49" s="1">
+      <c r="M49" s="1">
         <v>0.47630648347739302</v>
       </c>
-      <c r="L49" s="1">
+      <c r="N49" s="1">
         <v>2.1819999999999999</v>
       </c>
-      <c r="M49" s="1">
+      <c r="O49" s="1">
         <v>1.8407085737285198E-2</v>
       </c>
-      <c r="N49" s="2">
-        <v>1</v>
-      </c>
-      <c r="O49" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P49" s="3">
+      <c r="P49" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q49" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R49" s="3">
         <v>0.2</v>
       </c>
-      <c r="Q49" s="3">
-        <v>0</v>
-      </c>
-      <c r="R49" s="3">
+      <c r="S49" s="3">
+        <v>0</v>
+      </c>
+      <c r="T49" s="3">
         <v>0.8</v>
       </c>
-      <c r="S49" s="4" t="s">
+      <c r="U49" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="T49" s="3" t="s">
+      <c r="V49" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="U49" s="3" t="s">
+      <c r="W49" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>56</v>
       </c>
@@ -4313,44 +4622,50 @@
       <c r="I50" s="5">
         <v>33.65</v>
       </c>
-      <c r="J50" s="1">
+      <c r="J50" s="2">
+        <v>55</v>
+      </c>
+      <c r="K50" s="2">
+        <v>1.010645</v>
+      </c>
+      <c r="L50" s="1">
         <v>2.9379254585506418</v>
       </c>
-      <c r="K50" s="1">
+      <c r="M50" s="1">
         <v>0.41408220000000001</v>
       </c>
-      <c r="L50" s="1">
+      <c r="N50" s="1">
         <v>4.07</v>
       </c>
-      <c r="M50" s="1">
+      <c r="O50" s="1">
         <v>5.2436890000000002E-3</v>
       </c>
-      <c r="N50" s="2">
-        <v>1</v>
-      </c>
-      <c r="O50" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P50" s="3">
+      <c r="P50" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q50" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R50" s="3">
         <v>0.2</v>
       </c>
-      <c r="Q50" s="3">
-        <v>0</v>
-      </c>
-      <c r="R50" s="3">
+      <c r="S50" s="3">
+        <v>0</v>
+      </c>
+      <c r="T50" s="3">
         <v>0.8</v>
       </c>
-      <c r="S50" s="4" t="s">
+      <c r="U50" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="T50" s="3" t="s">
+      <c r="V50" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="U50" s="3" t="s">
+      <c r="W50" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>57</v>
       </c>
@@ -4378,44 +4693,50 @@
       <c r="I51" s="5">
         <v>1.2166999999999999</v>
       </c>
-      <c r="J51" s="1">
+      <c r="J51" s="2">
+        <v>2</v>
+      </c>
+      <c r="K51" s="2">
+        <v>1</v>
+      </c>
+      <c r="L51" s="1">
         <v>1.6653732518029856</v>
       </c>
-      <c r="K51" s="1">
+      <c r="M51" s="1">
         <v>0.32964342489972998</v>
       </c>
-      <c r="L51" s="1">
+      <c r="N51" s="1">
         <v>1.7270000000000001</v>
       </c>
-      <c r="M51" s="1">
+      <c r="O51" s="1">
         <v>0.124377</v>
       </c>
-      <c r="N51" s="2">
-        <v>1</v>
-      </c>
-      <c r="O51" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P51" s="3">
+      <c r="P51" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q51" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R51" s="3">
         <v>0.3</v>
       </c>
-      <c r="Q51" s="3">
-        <v>0</v>
-      </c>
-      <c r="R51" s="3">
+      <c r="S51" s="3">
+        <v>0</v>
+      </c>
+      <c r="T51" s="3">
         <v>0.7</v>
       </c>
-      <c r="S51" s="4" t="s">
+      <c r="U51" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="T51" s="3" t="s">
+      <c r="V51" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="U51" s="3" t="s">
+      <c r="W51" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>58</v>
       </c>
@@ -4443,44 +4764,50 @@
       <c r="I52" s="5">
         <v>1.6667000000000001</v>
       </c>
-      <c r="J52" s="1">
+      <c r="J52" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="K52" s="2">
+        <v>1</v>
+      </c>
+      <c r="L52" s="1">
         <v>2.9712055133338739</v>
       </c>
-      <c r="K52" s="1">
+      <c r="M52" s="1">
         <v>0.66430248183910701</v>
       </c>
-      <c r="L52" s="1">
+      <c r="N52" s="1">
         <v>3.7309999999999999</v>
       </c>
-      <c r="M52" s="1">
+      <c r="O52" s="1">
         <v>3.902812421549709E-2</v>
       </c>
-      <c r="N52" s="2">
-        <v>1</v>
-      </c>
-      <c r="O52" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P52" s="3">
+      <c r="P52" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q52" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R52" s="3">
         <v>0.3</v>
       </c>
-      <c r="Q52" s="3">
-        <v>0</v>
-      </c>
-      <c r="R52" s="3">
+      <c r="S52" s="3">
+        <v>0</v>
+      </c>
+      <c r="T52" s="3">
         <v>0.7</v>
       </c>
-      <c r="S52" s="4" t="s">
+      <c r="U52" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="T52" s="3" t="s">
+      <c r="V52" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="U52" s="3" t="s">
+      <c r="W52" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>59</v>
       </c>
@@ -4508,44 +4835,50 @@
       <c r="I53" s="5">
         <v>9.0333000000000006</v>
       </c>
-      <c r="J53" s="1">
+      <c r="J53" s="2">
+        <v>9.5</v>
+      </c>
+      <c r="K53" s="2">
+        <v>1.005897</v>
+      </c>
+      <c r="L53" s="1">
         <v>2.0278029169885938</v>
       </c>
-      <c r="K53" s="1">
+      <c r="M53" s="1">
         <v>0.28485614589455482</v>
       </c>
-      <c r="L53" s="1">
+      <c r="N53" s="1">
         <v>2.1160000000000001</v>
       </c>
-      <c r="M53" s="1">
+      <c r="O53" s="1">
         <v>0.10978160568538001</v>
       </c>
-      <c r="N53" s="2">
-        <v>1</v>
-      </c>
-      <c r="O53" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P53" s="3">
+      <c r="P53" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q53" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R53" s="3">
         <v>0.3</v>
       </c>
-      <c r="Q53" s="3">
-        <v>0</v>
-      </c>
-      <c r="R53" s="3">
+      <c r="S53" s="3">
+        <v>0</v>
+      </c>
+      <c r="T53" s="3">
         <v>0.7</v>
       </c>
-      <c r="S53" s="4" t="s">
+      <c r="U53" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="T53" s="3" t="s">
+      <c r="V53" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="U53" s="3" t="s">
+      <c r="W53" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>60</v>
       </c>
@@ -4573,40 +4906,46 @@
       <c r="I54" s="5">
         <v>4.3167</v>
       </c>
-      <c r="J54" s="1">
+      <c r="J54" s="2">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="K54" s="2">
+        <v>1</v>
+      </c>
+      <c r="L54" s="1">
         <v>0.7047179577675029</v>
       </c>
-      <c r="K54" s="1">
+      <c r="M54" s="1">
         <v>0.61036449999999998</v>
       </c>
-      <c r="L54" s="1">
+      <c r="N54" s="1">
         <v>1.653</v>
       </c>
-      <c r="M54" s="1">
+      <c r="O54" s="1">
         <v>0.11429010000000001</v>
       </c>
-      <c r="N54" s="2">
-        <v>1</v>
-      </c>
-      <c r="O54" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P54" s="3">
+      <c r="P54" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q54" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R54" s="3">
         <v>0.3</v>
       </c>
-      <c r="Q54" s="3">
-        <v>0</v>
-      </c>
-      <c r="R54" s="3">
+      <c r="S54" s="3">
+        <v>0</v>
+      </c>
+      <c r="T54" s="3">
         <v>0.7</v>
       </c>
-      <c r="S54" s="4" t="s">
+      <c r="U54" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="T54" s="3" t="s">
+      <c r="V54" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="U54" s="3" t="s">
+      <c r="W54" s="3" t="s">
         <v>87</v>
       </c>
     </row>

</xml_diff>